<commit_message>
added incorrect grammar lists
</commit_message>
<xml_diff>
--- a/xls/incorrect/G1_LP_A.xlsx
+++ b/xls/incorrect/G1_LP_A.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="10050"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14115" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,102 +16,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="35">
+  <si>
+    <t>po</t>
+  </si>
+  <si>
+    <t>pe</t>
+  </si>
+  <si>
+    <t>ba</t>
+  </si>
   <si>
     <t>lo</t>
   </si>
   <si>
+    <t>fi</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>ri</t>
+  </si>
+  <si>
+    <t>ko</t>
+  </si>
+  <si>
     <t>fu</t>
   </si>
   <si>
-    <t>ba</t>
-  </si>
-  <si>
     <t>pa</t>
   </si>
   <si>
-    <t>pe</t>
+    <t>se</t>
+  </si>
+  <si>
+    <t>so</t>
+  </si>
+  <si>
+    <t>bo</t>
+  </si>
+  <si>
+    <t>te</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>la</t>
+  </si>
+  <si>
+    <t>le</t>
+  </si>
+  <si>
+    <t>ta</t>
+  </si>
+  <si>
+    <t>ne</t>
+  </si>
+  <si>
+    <t>we</t>
+  </si>
+  <si>
+    <t>ka</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>di</t>
+  </si>
+  <si>
+    <t>li</t>
+  </si>
+  <si>
+    <t>wa</t>
+  </si>
+  <si>
+    <t>ni</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>ki</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>ti</t>
   </si>
   <si>
     <t>pi</t>
   </si>
   <si>
-    <t>po</t>
-  </si>
-  <si>
-    <t>fi</t>
+    <t>fe</t>
   </si>
   <si>
     <t>fa</t>
   </si>
   <si>
-    <t>fe</t>
-  </si>
-  <si>
-    <t>we</t>
-  </si>
-  <si>
-    <t>wa</t>
-  </si>
-  <si>
-    <t>se</t>
-  </si>
-  <si>
-    <t>so</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>to</t>
-  </si>
-  <si>
-    <t>ta</t>
-  </si>
-  <si>
-    <t>te</t>
-  </si>
-  <si>
-    <t>ti</t>
-  </si>
-  <si>
-    <t>ki</t>
-  </si>
-  <si>
-    <t>ka</t>
-  </si>
-  <si>
-    <t>ko</t>
-  </si>
-  <si>
     <t>ra</t>
-  </si>
-  <si>
-    <t>ri</t>
-  </si>
-  <si>
-    <t>be</t>
-  </si>
-  <si>
-    <t>bo</t>
-  </si>
-  <si>
-    <t>di</t>
-  </si>
-  <si>
-    <t>do</t>
-  </si>
-  <si>
-    <t>ni</t>
-  </si>
-  <si>
-    <t>mi</t>
-  </si>
-  <si>
-    <t>la</t>
-  </si>
-  <si>
-    <t>le</t>
   </si>
 </sst>
 </file>
@@ -452,994 +461,994 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" zoomScaleNormal="62" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H1">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I1">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J1">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K1">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L1">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M1">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I2">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J2">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K2">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L2">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M2">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
       <c r="H3">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I3">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J3">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K3">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L3">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M3">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>51</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I4">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J4">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K4">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L4">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M4">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
       <c r="G5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I5">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J5">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K5">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L5">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M5">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>15</v>
-      </c>
       <c r="G6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I6">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J6">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K6">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L6">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M6">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H7">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I7">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J7">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K7">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L7">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M7">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
         <v>2</v>
       </c>
       <c r="H8">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I8">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J8">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K8">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L8">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M8">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H9">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I9">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J9">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K9">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L9">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M9">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>43</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="G10" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="H10">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I10">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J10">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K10">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L10">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M10">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>55</v>
+        <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H11">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I11">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J11">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K11">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L11">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M11">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H12">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I12">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J12">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K12">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L12">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M12">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H13">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I13">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J13">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K13">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L13">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M13">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G14" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H14">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I14">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J14">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K14">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L14">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M14">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>0</v>
-      </c>
       <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
         <v>20</v>
       </c>
-      <c r="E15" t="s">
-        <v>1</v>
-      </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G15" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H15">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I15">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J15">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K15">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L15">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M15">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E16" t="s">
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="G16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H16">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I16">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J16">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K16">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L16">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M16">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
+        <v>5</v>
+      </c>
+      <c r="F17" t="s">
         <v>1</v>
       </c>
-      <c r="F17" t="s">
-        <v>15</v>
-      </c>
       <c r="G17" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H17">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I17">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J17">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K17">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L17">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M17">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="E18" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G18" t="s">
         <v>2</v>
       </c>
       <c r="H18">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I18">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J18">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K18">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L18">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M18">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
         <v>4</v>
       </c>
-      <c r="C19" t="s">
-        <v>0</v>
-      </c>
       <c r="D19" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H19">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I19">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J19">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K19">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L19">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M19">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>22</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" t="s">
-        <v>1</v>
-      </c>
-      <c r="F20" t="s">
-        <v>15</v>
-      </c>
       <c r="G20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H20">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I20">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J20">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K20">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L20">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M20">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>46</v>
+        <v>27</v>
       </c>
       <c r="B21" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C21" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G21" t="s">
         <v>2</v>
       </c>
       <c r="H21">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I21">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J21">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K21">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L21">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M21">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="B22" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G22" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H22">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I22">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J22">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K22">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L22">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M22">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C23" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G23" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H23">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I23">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J23">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K23">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L23">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M23">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C24" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="E24" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" t="s">
         <v>1</v>
       </c>
-      <c r="F24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" t="s">
-        <v>2</v>
-      </c>
       <c r="H24">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I24">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J24">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K24">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L24">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M24">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1447,655 +1456,655 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="C25" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G25" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H25">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I25">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J25">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K25">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L25">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M25">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
-        <v>0</v>
-      </c>
-      <c r="D26" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" t="s">
-        <v>1</v>
-      </c>
-      <c r="F26" t="s">
-        <v>15</v>
-      </c>
       <c r="G26" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H26">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I26">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J26">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K26">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L26">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M26">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B27" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="E27" t="s">
         <v>1</v>
       </c>
       <c r="F27" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G27" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H27">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I27">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J27">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K27">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L27">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M27">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C28" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G28" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H28">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I28">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J28">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K28">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L28">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M28">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="B29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D29" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H29">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I29">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J29">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K29">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L29">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M29">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>25</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>0</v>
-      </c>
-      <c r="D30" t="s">
-        <v>17</v>
-      </c>
-      <c r="E30" t="s">
-        <v>1</v>
-      </c>
       <c r="F30" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="G30" t="s">
         <v>2</v>
       </c>
       <c r="H30">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I30">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J30">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K30">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L30">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M30">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" t="s">
+        <v>28</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" t="s">
         <v>29</v>
       </c>
-      <c r="E31" t="s">
-        <v>1</v>
-      </c>
-      <c r="F31" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" t="s">
-        <v>2</v>
-      </c>
       <c r="H31">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I31">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J31">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K31">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L31">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M31">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
         <v>4</v>
       </c>
-      <c r="C32" t="s">
-        <v>0</v>
-      </c>
       <c r="D32" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E32" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G32" t="s">
         <v>2</v>
       </c>
       <c r="H32">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I32">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J32">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K32">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L32">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M32">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D33" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="E33" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G33" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H33">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I33">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J33">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K33">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L33">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M33">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
       <c r="F34" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="G34" t="s">
         <v>2</v>
       </c>
       <c r="H34">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I34">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J34">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K34">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L34">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M34">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="C35" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D35" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="E35" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="G35" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H35">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I35">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J35">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K35">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L35">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M35">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B36" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C36" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="G36" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="H36">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I36">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J36">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K36">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L36">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M36">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="E37" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F37" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="G37" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H37">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I37">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J37">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K37">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L37">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M37">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" t="s">
+        <v>3</v>
+      </c>
+      <c r="E38" t="s">
         <v>4</v>
       </c>
-      <c r="C38" t="s">
-        <v>0</v>
-      </c>
-      <c r="D38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" t="s">
-        <v>1</v>
-      </c>
       <c r="F38" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G38" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H38">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I38">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J38">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K38">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L38">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M38">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C39" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D39" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E39" t="s">
         <v>1</v>
       </c>
       <c r="F39" t="s">
+        <v>8</v>
+      </c>
+      <c r="G39" t="s">
         <v>15</v>
       </c>
-      <c r="G39" t="s">
-        <v>2</v>
-      </c>
       <c r="H39">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I39">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J39">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K39">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L39">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M39">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C40" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="G40" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H40">
-        <v>11</v>
+        <v>111</v>
       </c>
       <c r="I40">
-        <v>12</v>
+        <v>112</v>
       </c>
       <c r="J40">
-        <v>21</v>
+        <v>121</v>
       </c>
       <c r="K40">
-        <v>22</v>
+        <v>122</v>
       </c>
       <c r="L40">
-        <v>31</v>
+        <v>131</v>
       </c>
       <c r="M40">
-        <v>32</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated and removed files - added new scale 1-5 rating of confidence for test phase
</commit_message>
<xml_diff>
--- a/xls/incorrect/G1_LP_A.xlsx
+++ b/xls/incorrect/G1_LP_A.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -462,7 +462,7 @@
   <dimension ref="A1:M40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -595,22 +595,22 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
       </c>
       <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
         <v>4</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>3</v>
       </c>
       <c r="H4">
         <v>111</v>
@@ -639,19 +639,19 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F5" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H5">
         <v>111</v>
@@ -771,7 +771,7 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G8" t="s">
         <v>2</v>
@@ -800,10 +800,10 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -929,10 +929,10 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -1087,22 +1087,22 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
         <v>5</v>
       </c>
-      <c r="D16" t="s">
-        <v>8</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="G16" t="s">
         <v>1</v>
-      </c>
-      <c r="F16" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>5</v>
       </c>
       <c r="H16">
         <v>111</v>
@@ -1175,16 +1175,16 @@
         <v>2</v>
       </c>
       <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
         <v>5</v>
       </c>
-      <c r="E18" t="s">
-        <v>8</v>
-      </c>
       <c r="F18" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G18" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H18">
         <v>111</v>
@@ -1427,10 +1427,10 @@
         <v>8</v>
       </c>
       <c r="F24" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G24" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="H24">
         <v>111</v>
@@ -1503,7 +1503,7 @@
         <v>21</v>
       </c>
       <c r="D26" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -1588,10 +1588,10 @@
         <v>8</v>
       </c>
       <c r="E28" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F28" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G28" t="s">
         <v>8</v>
@@ -1673,7 +1673,7 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G30" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
corrected incorrect lists ;)
</commit_message>
<xml_diff>
--- a/xls/incorrect/G1_LP_A.xlsx
+++ b/xls/incorrect/G1_LP_A.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14115" windowHeight="6735"/>
+    <workbookView xWindow="150" yWindow="90" windowWidth="8505" windowHeight="6735"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525" concurrentCalc="0"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -595,19 +595,19 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
       <c r="F4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
         <v>4</v>
@@ -639,16 +639,16 @@
         <v>2</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
@@ -724,10 +724,10 @@
         <v>13</v>
       </c>
       <c r="D7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" t="s">
         <v>14</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
       </c>
       <c r="F7" t="s">
         <v>2</v>
@@ -771,7 +771,7 @@
         <v>3</v>
       </c>
       <c r="F8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G8" t="s">
         <v>2</v>
@@ -800,10 +800,10 @@
         <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -841,19 +841,19 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D10" t="s">
         <v>1</v>
       </c>
       <c r="E10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" t="s">
         <v>4</v>
-      </c>
-      <c r="F10" t="s">
-        <v>16</v>
       </c>
       <c r="G10" t="s">
         <v>17</v>
@@ -929,10 +929,10 @@
         <v>5</v>
       </c>
       <c r="D12" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F12" t="s">
         <v>10</v>
@@ -1087,22 +1087,22 @@
         <v>25</v>
       </c>
       <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" t="s">
         <v>5</v>
       </c>
-      <c r="C16" t="s">
-        <v>10</v>
-      </c>
       <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
         <v>1</v>
       </c>
-      <c r="E16" t="s">
-        <v>8</v>
-      </c>
       <c r="F16" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
         <v>5</v>
-      </c>
-      <c r="G16" t="s">
-        <v>1</v>
       </c>
       <c r="H16">
         <v>111</v>
@@ -1219,13 +1219,13 @@
         <v>8</v>
       </c>
       <c r="E19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" t="s">
         <v>4</v>
       </c>
-      <c r="F19" t="s">
-        <v>2</v>
-      </c>
       <c r="G19" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="H19">
         <v>111</v>
@@ -1251,22 +1251,22 @@
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C20" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
         <v>3</v>
       </c>
       <c r="F20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H20">
         <v>111</v>
@@ -1380,13 +1380,13 @@
         <v>3</v>
       </c>
       <c r="D23" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E23" t="s">
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G23" t="s">
         <v>8</v>
@@ -1415,7 +1415,7 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C24" t="s">
         <v>5</v>
@@ -1424,13 +1424,13 @@
         <v>2</v>
       </c>
       <c r="E24" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G24" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H24">
         <v>111</v>
@@ -1497,13 +1497,13 @@
         <v>44</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C26" t="s">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="E26" t="s">
         <v>7</v>
@@ -1512,7 +1512,7 @@
         <v>4</v>
       </c>
       <c r="G26" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H26">
         <v>111</v>
@@ -1538,19 +1538,19 @@
         <v>15</v>
       </c>
       <c r="B27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
         <v>24</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1</v>
       </c>
       <c r="D27" t="s">
         <v>11</v>
       </c>
       <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
         <v>1</v>
-      </c>
-      <c r="F27" t="s">
-        <v>2</v>
       </c>
       <c r="G27" t="s">
         <v>10</v>
@@ -1579,19 +1579,19 @@
         <v>1</v>
       </c>
       <c r="B28" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+      <c r="E28" t="s">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
-        <v>3</v>
-      </c>
-      <c r="D28" t="s">
-        <v>8</v>
-      </c>
-      <c r="E28" t="s">
-        <v>23</v>
-      </c>
       <c r="F28" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="G28" t="s">
         <v>8</v>
@@ -1673,7 +1673,7 @@
         <v>25</v>
       </c>
       <c r="F30" t="s">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G30" t="s">
         <v>2</v>
@@ -1708,10 +1708,10 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" t="s">
         <v>4</v>
-      </c>
-      <c r="E31" t="s">
-        <v>28</v>
       </c>
       <c r="F31" t="s">
         <v>8</v>
@@ -1749,13 +1749,13 @@
         <v>4</v>
       </c>
       <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
         <v>30</v>
-      </c>
-      <c r="E32" t="s">
-        <v>3</v>
-      </c>
-      <c r="F32" t="s">
-        <v>2</v>
       </c>
       <c r="G32" t="s">
         <v>2</v>
@@ -1787,7 +1787,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="D33" t="s">
         <v>4</v>
@@ -1796,10 +1796,10 @@
         <v>2</v>
       </c>
       <c r="F33" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G33" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H33">
         <v>111</v>
@@ -1828,7 +1828,7 @@
         <v>10</v>
       </c>
       <c r="C34" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D34" t="s">
         <v>3</v>
@@ -1837,7 +1837,7 @@
         <v>31</v>
       </c>
       <c r="F34" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G34" t="s">
         <v>2</v>
@@ -1913,13 +1913,13 @@
         <v>33</v>
       </c>
       <c r="D36" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G36" t="s">
         <v>23</v>
@@ -1951,16 +1951,16 @@
         <v>22</v>
       </c>
       <c r="C37" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D37" t="s">
         <v>4</v>
       </c>
       <c r="E37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
         <v>4</v>
-      </c>
-      <c r="F37" t="s">
-        <v>3</v>
       </c>
       <c r="G37" t="s">
         <v>8</v>
@@ -1992,10 +1992,10 @@
         <v>34</v>
       </c>
       <c r="C38" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D38" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="E38" t="s">
         <v>4</v>
@@ -2071,7 +2071,7 @@
         <v>12</v>
       </c>
       <c r="B40" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
@@ -2083,7 +2083,7 @@
         <v>8</v>
       </c>
       <c r="F40" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G40" t="s">
         <v>3</v>

</xml_diff>